<commit_message>
Added default catch all option
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randeep.siddhu/pubmatic/source/tools/create_mediaconfig/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randeep.siddhu/pubmatic/source/tools/createmediaconfig/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9D0D9D-472A-EF4D-9F93-C7AEE54F7BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06722BC3-08D6-B349-A8B4-F8C6A26576A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58200" yWindow="-3400" windowWidth="25980" windowHeight="23120" xr2:uid="{E0846DB2-500E-A144-8641-2AE03101976A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="17640" windowHeight="20160" xr2:uid="{E0846DB2-500E-A144-8641-2AE03101976A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>AdUnit</t>
   </si>
@@ -44,83 +44,68 @@
     <t>OWFloor</t>
   </si>
   <si>
-    <t>max_wy_android_banner_1</t>
-  </si>
-  <si>
-    <t>max_wy_android_banner_2</t>
-  </si>
-  <si>
-    <t>max_wy_android_banner_3</t>
-  </si>
-  <si>
-    <t>max_wy_android_banner_4</t>
-  </si>
-  <si>
-    <t>max_wy_android_interstitial_1</t>
-  </si>
-  <si>
-    <t>max_wy_android_interstitial_2</t>
-  </si>
-  <si>
-    <t>max_wy_android_interstitial_3</t>
-  </si>
-  <si>
-    <t>max_wy_android_interstitial_4</t>
-  </si>
-  <si>
-    <t>max_wy_android_rewarded_1</t>
-  </si>
-  <si>
-    <t>max_wy_android_rewarded_2</t>
-  </si>
-  <si>
-    <t>max_wy_android_rewarded_3</t>
-  </si>
-  <si>
-    <t>max_wy_android_rewarded_4</t>
-  </si>
-  <si>
-    <t>max_wy_ios_banner_1</t>
-  </si>
-  <si>
-    <t>max_wy_ios_banner_2</t>
-  </si>
-  <si>
-    <t>max_wy_ios_banner_3</t>
-  </si>
-  <si>
-    <t>max_wy_ios_banner_4</t>
-  </si>
-  <si>
-    <t>max_wy_ios_interstitial_1</t>
-  </si>
-  <si>
-    <t>max_wy_ios_interstitial_2</t>
-  </si>
-  <si>
-    <t>max_wy_ios_interstitial_3</t>
-  </si>
-  <si>
-    <t>max_wy_ios_interstitial_4</t>
-  </si>
-  <si>
-    <t>max_wy_ios_rewarded_1</t>
-  </si>
-  <si>
-    <t>max_wy_ios_rewarded_2</t>
-  </si>
-  <si>
-    <t>max_wy_ios_rewarded_3</t>
-  </si>
-  <si>
-    <t>max_wy_ios_rewarded_4</t>
+    <t>OW_And_banner_0</t>
+  </si>
+  <si>
+    <t>OW_And_banner_1</t>
+  </si>
+  <si>
+    <t>OW_And_banner_2</t>
+  </si>
+  <si>
+    <t>OW_And_banner_3</t>
+  </si>
+  <si>
+    <t>OW_And_Inter_0</t>
+  </si>
+  <si>
+    <t>OW_And_Inter_1</t>
+  </si>
+  <si>
+    <t>OW_And_Inter_2</t>
+  </si>
+  <si>
+    <t>OW_And_Inter_3</t>
+  </si>
+  <si>
+    <t>OW_And_Inter_4</t>
+  </si>
+  <si>
+    <t>OW_iOS_banner_0</t>
+  </si>
+  <si>
+    <t>OW_iOS_banner_1</t>
+  </si>
+  <si>
+    <t>OW_iOS_banner_2</t>
+  </si>
+  <si>
+    <t>OW_iOS_banner_3</t>
+  </si>
+  <si>
+    <t>OW_iOS_Inter_0</t>
+  </si>
+  <si>
+    <t>OW_iOS_Inter_1</t>
+  </si>
+  <si>
+    <t>OW_iOS_Inter_2</t>
+  </si>
+  <si>
+    <t>OW_iOS_Inter_3</t>
+  </si>
+  <si>
+    <t>OW_iOS_Inter_4</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,12 +118,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF212121"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -173,11 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,15 +470,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B46C106-7ADF-F141-BD06-4A5E73D957CE}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="41.5" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -512,244 +490,156 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="B11" s="1">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>